<commit_message>
3rd semester final projects
</commit_message>
<xml_diff>
--- a/3.2.CaracterizacionDeMateriales/10_FinalProject/colabGrading.xlsx
+++ b/3.2.CaracterizacionDeMateriales/10_FinalProject/colabGrading.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecmx-my.sharepoint.com/personal/a01212611_itesm_mx/Documents/Documents/MNT_ITESM_courses/3.2.CaracterizacionDeMateriales/11_colab_grading/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecmx-my.sharepoint.com/personal/a01212611_itesm_mx/Documents/Documents/MNT_ITESM_courses/3.2.CaracterizacionDeMateriales/10_FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{64680DE5-806C-4BF7-B540-7638547001CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CE9B304C-D31F-4A25-8BE6-A2767433544A}"/>
+  <xr:revisionPtr revIDLastSave="275" documentId="8_{64680DE5-806C-4BF7-B540-7638547001CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3A1DA567-C47C-4223-ACDD-383353ED0DA2}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="18555" windowHeight="9135" xr2:uid="{41796C17-581F-44C5-8E95-B5CC6C9AC82A}"/>
+    <workbookView xWindow="900" yWindow="2160" windowWidth="18555" windowHeight="11835" xr2:uid="{41796C17-581F-44C5-8E95-B5CC6C9AC82A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+  <si>
+    <t>https://forms.gle/rfmhozfBwD2LqXv37</t>
+  </si>
+  <si>
+    <t>title:</t>
+  </si>
+  <si>
+    <t>Characterization of PLA/TiO2 NPs for Biomedical Applications</t>
+  </si>
+  <si>
+    <t>Fabrication of Antibacterial Chitosan-Polystyrene Blended Film Using Electrospray and Plasma Surface Modification for Food Packaging Applications</t>
+  </si>
+  <si>
+    <t>Ni-Al2O3 Coating on Low Carbon Steel (and more!)</t>
+  </si>
+  <si>
+    <t>Characterization of GelMA-Based Core-Shell Microgel Fabricated by Droplet Microfluidic System</t>
+  </si>
+  <si>
+    <t>Nanostructured Lipid Carriers Loaded with Vitamin A as Anti-Aging Precursor for Cosmetic Applications</t>
+  </si>
+  <si>
+    <t>Characterization of nHap-Polymer Composite Fibers for Bone Tissue Engineering</t>
+  </si>
+  <si>
+    <t>Carbon nano-onions reinforced nanocomposites</t>
+  </si>
+  <si>
+    <t>presentation no.:</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
   <si>
     <t>introduction:</t>
   </si>
@@ -41,6 +74,12 @@
     <t>justification:</t>
   </si>
   <si>
+    <t>sample preparation:</t>
+  </si>
+  <si>
+    <t>applicartion of methods:</t>
+  </si>
+  <si>
     <t>analysis:</t>
   </si>
   <si>
@@ -53,43 +92,22 @@
     <t>knowledge:</t>
   </si>
   <si>
-    <t>sample preparation:</t>
-  </si>
-  <si>
-    <t>applicartion of methods:</t>
-  </si>
-  <si>
     <t>total:</t>
   </si>
   <si>
-    <t>Characterization of PLA/TiO2 NPs for Biomedical Applications</t>
-  </si>
-  <si>
-    <t>Fabrication of Antibacterial Chitosan-Polystyrene Blended Film Using Electrospray and Plasma Surface Modification for Food Packaging Applications</t>
-  </si>
-  <si>
-    <t>Ni-Al2O3 Coating on Low Carbon Steel (and more!)</t>
-  </si>
-  <si>
-    <t>Characterization of GelMA-Based Core-Shell Microgel Fabricated by Droplet Microfluidic System</t>
-  </si>
-  <si>
-    <t>Nanostructured Lipid Carriers Loaded with Vitamin A as Anti-Aging Precursor for Cosmetic Applications</t>
-  </si>
-  <si>
-    <t>Characterization of nHap-Polymer Composite Fibers for Bone Tissue Engineering</t>
-  </si>
-  <si>
-    <t>avg</t>
-  </si>
-  <si>
-    <t>https://forms.gle/rfmhozfBwD2LqXv37</t>
-  </si>
-  <si>
-    <t>title:</t>
-  </si>
-  <si>
-    <t>presentation no.:</t>
+    <t>Proposal of Characterization Procedure of A PCLC SIROLIMUS-ELUTING Mg-STENT</t>
+  </si>
+  <si>
+    <t>[video] Characterization of Carbon Fiber Composites Adding CNTs with epoxy Matrix for Industrial Applications</t>
+  </si>
+  <si>
+    <t>Fiber reinforced concrete for 3D printing applications</t>
+  </si>
+  <si>
+    <t>1st DAY</t>
+  </si>
+  <si>
+    <t>2nd DAY</t>
   </si>
 </sst>
 </file>
@@ -182,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -198,6 +216,9 @@
     <xf numFmtId="1" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -513,10 +534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C1272E-C6B5-44FF-B5FE-D147CD89F482}">
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:AT12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <pane xSplit="1" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AT3" sqref="AT3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,55 +547,93 @@
     <col min="2" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
+      <c r="Z2" s="14" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="AD2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="14" t="str">
+        <f>""</f>
+        <v/>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -585,7 +645,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3">
         <v>2</v>
@@ -597,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J3" s="4">
         <v>3</v>
@@ -609,7 +669,7 @@
         <v>3</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N3" s="5">
         <v>4</v>
@@ -621,7 +681,7 @@
         <v>4</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="R3" s="6">
         <v>5</v>
@@ -633,7 +693,7 @@
         <v>5</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="V3" s="1">
         <v>6</v>
@@ -645,12 +705,60 @@
         <v>6</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="3">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="3">
+        <v>2</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL3" s="4">
+        <v>4</v>
+      </c>
+      <c r="AM3" s="4">
+        <v>4</v>
+      </c>
+      <c r="AN3" s="4">
+        <v>4</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AR3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AS3" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B4" s="7">
         <v>10</v>
@@ -730,10 +838,62 @@
         <f>AVERAGE(V4:X4)</f>
         <v>10</v>
       </c>
+      <c r="AD4" s="2">
+        <v>10</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>10</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>10</v>
+      </c>
+      <c r="AG4" s="2">
+        <f>AVERAGE(AD4:AF4)</f>
+        <v>10</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>10</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>10</v>
+      </c>
+      <c r="AJ4" s="3">
+        <v>10</v>
+      </c>
+      <c r="AK4" s="3">
+        <f>AVERAGE(AH4:AJ4)</f>
+        <v>10</v>
+      </c>
+      <c r="AL4" s="4">
+        <v>10</v>
+      </c>
+      <c r="AM4" s="4">
+        <v>10</v>
+      </c>
+      <c r="AN4" s="4">
+        <v>10</v>
+      </c>
+      <c r="AO4" s="4">
+        <f>AVERAGE(AL4:AN4)</f>
+        <v>10</v>
+      </c>
+      <c r="AP4" s="5">
+        <v>10</v>
+      </c>
+      <c r="AQ4" s="5">
+        <v>10</v>
+      </c>
+      <c r="AR4" s="5">
+        <v>10</v>
+      </c>
+      <c r="AS4" s="5">
+        <f>AVERAGE(AP4:AR4)</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B5" s="7">
         <v>15</v>
@@ -813,10 +973,62 @@
         <f t="shared" ref="Y5:Y12" si="5">AVERAGE(V5:X5)</f>
         <v>14.666666666666666</v>
       </c>
+      <c r="AD5" s="2">
+        <v>13</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>14</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>15</v>
+      </c>
+      <c r="AG5" s="2">
+        <f>AVERAGE(AD5:AF5)</f>
+        <v>14</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>15</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>15</v>
+      </c>
+      <c r="AJ5" s="3">
+        <v>15</v>
+      </c>
+      <c r="AK5" s="3">
+        <f>AVERAGE(AH5:AJ5)</f>
+        <v>15</v>
+      </c>
+      <c r="AL5" s="4">
+        <v>15</v>
+      </c>
+      <c r="AM5" s="4">
+        <v>15</v>
+      </c>
+      <c r="AN5" s="4">
+        <v>15</v>
+      </c>
+      <c r="AO5" s="4">
+        <f>AVERAGE(AL5:AN5)</f>
+        <v>15</v>
+      </c>
+      <c r="AP5" s="5">
+        <v>15</v>
+      </c>
+      <c r="AQ5" s="5">
+        <v>15</v>
+      </c>
+      <c r="AR5" s="5">
+        <v>15</v>
+      </c>
+      <c r="AS5" s="5">
+        <f>AVERAGE(AP5:AR5)</f>
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B6" s="7">
         <v>10</v>
@@ -896,10 +1108,62 @@
         <f t="shared" si="5"/>
         <v>9.3333333333333339</v>
       </c>
+      <c r="AD6" s="2">
+        <v>9</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>9</v>
+      </c>
+      <c r="AF6" s="2">
+        <v>10</v>
+      </c>
+      <c r="AG6" s="2">
+        <f>AVERAGE(AD6:AF6)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>10</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>10</v>
+      </c>
+      <c r="AJ6" s="3">
+        <v>10</v>
+      </c>
+      <c r="AK6" s="3">
+        <f>AVERAGE(AH6:AJ6)</f>
+        <v>10</v>
+      </c>
+      <c r="AL6" s="4">
+        <v>10</v>
+      </c>
+      <c r="AM6" s="4">
+        <v>10</v>
+      </c>
+      <c r="AN6" s="4">
+        <v>10</v>
+      </c>
+      <c r="AO6" s="4">
+        <f>AVERAGE(AL6:AN6)</f>
+        <v>10</v>
+      </c>
+      <c r="AP6" s="5">
+        <v>9</v>
+      </c>
+      <c r="AQ6" s="5">
+        <v>8</v>
+      </c>
+      <c r="AR6" s="5">
+        <v>10</v>
+      </c>
+      <c r="AS6" s="5">
+        <f>AVERAGE(AP6:AR6)</f>
+        <v>9</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B7" s="7">
         <v>14</v>
@@ -979,10 +1243,62 @@
         <f t="shared" si="5"/>
         <v>14.666666666666666</v>
       </c>
+      <c r="AD7" s="2">
+        <v>14</v>
+      </c>
+      <c r="AE7" s="2">
+        <v>14</v>
+      </c>
+      <c r="AF7" s="2">
+        <v>15</v>
+      </c>
+      <c r="AG7" s="2">
+        <f>AVERAGE(AD7:AF7)</f>
+        <v>14.333333333333334</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>15</v>
+      </c>
+      <c r="AI7" s="3">
+        <v>15</v>
+      </c>
+      <c r="AJ7" s="3">
+        <v>15</v>
+      </c>
+      <c r="AK7" s="3">
+        <f>AVERAGE(AH7:AJ7)</f>
+        <v>15</v>
+      </c>
+      <c r="AL7" s="4">
+        <v>14</v>
+      </c>
+      <c r="AM7" s="4">
+        <v>13</v>
+      </c>
+      <c r="AN7" s="4">
+        <v>15</v>
+      </c>
+      <c r="AO7" s="4">
+        <f>AVERAGE(AL7:AN7)</f>
+        <v>14</v>
+      </c>
+      <c r="AP7" s="5">
+        <v>15</v>
+      </c>
+      <c r="AQ7" s="5">
+        <v>15</v>
+      </c>
+      <c r="AR7" s="5">
+        <v>15</v>
+      </c>
+      <c r="AS7" s="5">
+        <f>AVERAGE(AP7:AR7)</f>
+        <v>15</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B8" s="7">
         <v>14</v>
@@ -1062,10 +1378,62 @@
         <f t="shared" si="5"/>
         <v>14.666666666666666</v>
       </c>
+      <c r="AD8" s="2">
+        <v>14</v>
+      </c>
+      <c r="AE8" s="2">
+        <v>14</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>15</v>
+      </c>
+      <c r="AG8" s="2">
+        <f>AVERAGE(AD8:AF8)</f>
+        <v>14.333333333333334</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>14</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>14</v>
+      </c>
+      <c r="AJ8" s="3">
+        <v>15</v>
+      </c>
+      <c r="AK8" s="3">
+        <f>AVERAGE(AH8:AJ8)</f>
+        <v>14.333333333333334</v>
+      </c>
+      <c r="AL8" s="4">
+        <v>14</v>
+      </c>
+      <c r="AM8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AN8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AO8" s="4">
+        <f>AVERAGE(AL8:AN8)</f>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="AP8" s="5">
+        <v>15</v>
+      </c>
+      <c r="AQ8" s="5">
+        <v>15</v>
+      </c>
+      <c r="AR8" s="5">
+        <v>15</v>
+      </c>
+      <c r="AS8" s="5">
+        <f>AVERAGE(AP8:AR8)</f>
+        <v>15</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B9" s="7">
         <v>10</v>
@@ -1145,10 +1513,62 @@
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
+      <c r="AD9" s="2">
+        <v>10</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>10</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>10</v>
+      </c>
+      <c r="AG9" s="2">
+        <f>AVERAGE(AD9:AF9)</f>
+        <v>10</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>10</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>10</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>10</v>
+      </c>
+      <c r="AK9" s="3">
+        <f>AVERAGE(AH9:AJ9)</f>
+        <v>10</v>
+      </c>
+      <c r="AL9" s="4">
+        <v>10</v>
+      </c>
+      <c r="AM9" s="4">
+        <v>10</v>
+      </c>
+      <c r="AN9" s="4">
+        <v>10</v>
+      </c>
+      <c r="AO9" s="4">
+        <f>AVERAGE(AL9:AN9)</f>
+        <v>10</v>
+      </c>
+      <c r="AP9" s="5">
+        <v>10</v>
+      </c>
+      <c r="AQ9" s="5">
+        <v>10</v>
+      </c>
+      <c r="AR9" s="5">
+        <v>10</v>
+      </c>
+      <c r="AS9" s="5">
+        <f>AVERAGE(AP9:AR9)</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B10" s="7">
         <v>10</v>
@@ -1228,10 +1648,62 @@
         <f t="shared" si="5"/>
         <v>9.6666666666666661</v>
       </c>
+      <c r="AD10" s="2">
+        <v>9</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>9</v>
+      </c>
+      <c r="AF10" s="2">
+        <v>10</v>
+      </c>
+      <c r="AG10" s="2">
+        <f>AVERAGE(AD10:AF10)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>10</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>10</v>
+      </c>
+      <c r="AJ10" s="3">
+        <v>10</v>
+      </c>
+      <c r="AK10" s="3">
+        <f>AVERAGE(AH10:AJ10)</f>
+        <v>10</v>
+      </c>
+      <c r="AL10" s="4">
+        <v>9</v>
+      </c>
+      <c r="AM10" s="4">
+        <v>9</v>
+      </c>
+      <c r="AN10" s="4">
+        <v>10</v>
+      </c>
+      <c r="AO10" s="4">
+        <f>AVERAGE(AL10:AN10)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="AP10" s="5">
+        <v>10</v>
+      </c>
+      <c r="AQ10" s="5">
+        <v>10</v>
+      </c>
+      <c r="AR10" s="5">
+        <v>10</v>
+      </c>
+      <c r="AS10" s="5">
+        <f>AVERAGE(AP10:AR10)</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B11" s="7">
         <v>15</v>
@@ -1311,10 +1783,62 @@
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
+      <c r="AD11" s="2">
+        <v>14</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>13</v>
+      </c>
+      <c r="AF11" s="2">
+        <v>15</v>
+      </c>
+      <c r="AG11" s="2">
+        <f>AVERAGE(AD11:AF11)</f>
+        <v>14</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>15</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>14</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>15</v>
+      </c>
+      <c r="AK11" s="3">
+        <f>AVERAGE(AH11:AJ11)</f>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="AL11" s="4">
+        <v>15</v>
+      </c>
+      <c r="AM11" s="4">
+        <v>15</v>
+      </c>
+      <c r="AN11" s="4">
+        <v>15</v>
+      </c>
+      <c r="AO11" s="4">
+        <f>AVERAGE(AL11:AN11)</f>
+        <v>15</v>
+      </c>
+      <c r="AP11" s="5">
+        <v>15</v>
+      </c>
+      <c r="AQ11" s="5">
+        <v>15</v>
+      </c>
+      <c r="AR11" s="5">
+        <v>15</v>
+      </c>
+      <c r="AS11" s="5">
+        <f>AVERAGE(AP11:AR11)</f>
+        <v>15</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B12" s="7">
         <f>SUM(B4:B11)</f>
@@ -1412,8 +1936,75 @@
         <f t="shared" si="5"/>
         <v>98</v>
       </c>
+      <c r="AD12" s="2">
+        <f>SUM(AD4:AD11)</f>
+        <v>93</v>
+      </c>
+      <c r="AE12" s="2">
+        <f t="shared" ref="AE12:AS12" si="9">SUM(AE4:AE11)</f>
+        <v>93</v>
+      </c>
+      <c r="AF12" s="2">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="AG12" s="2">
+        <f t="shared" si="9"/>
+        <v>95.333333333333329</v>
+      </c>
+      <c r="AH12" s="3">
+        <f t="shared" si="9"/>
+        <v>99</v>
+      </c>
+      <c r="AI12" s="3">
+        <f t="shared" si="9"/>
+        <v>98</v>
+      </c>
+      <c r="AJ12" s="3">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="AK12" s="3">
+        <f t="shared" si="9"/>
+        <v>99</v>
+      </c>
+      <c r="AL12" s="4">
+        <f t="shared" si="9"/>
+        <v>97</v>
+      </c>
+      <c r="AM12" s="4">
+        <f t="shared" si="9"/>
+        <v>97</v>
+      </c>
+      <c r="AN12" s="4">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="AO12" s="4">
+        <f t="shared" si="9"/>
+        <v>97.999999999999986</v>
+      </c>
+      <c r="AP12" s="5">
+        <f t="shared" si="9"/>
+        <v>99</v>
+      </c>
+      <c r="AQ12" s="5">
+        <f t="shared" si="9"/>
+        <v>98</v>
+      </c>
+      <c r="AR12" s="5">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="AS12" s="5">
+        <f t="shared" si="9"/>
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AD2:AG2"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{B93F3C85-4973-43DA-AF4E-0A093E6E0B4B}"/>
   </hyperlinks>
@@ -1690,16 +2281,8 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32A9C241-A8C5-404E-AB94-9C26CD60C024}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e2309a97-5dbe-4782-af0a-c6fa888d645b"/>
-    <ds:schemaRef ds:uri="faf185f4-fa7c-4454-b7fc-1060ac3b9dc2"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>